<commit_message>
Fixed issue with string concatenation in excel_utils.py
</commit_message>
<xml_diff>
--- a/data_new.xlsx
+++ b/data_new.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,22 +451,22 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Prajwal</t>
+          <t>pramod</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>09036409517</t>
+          <t>563456235263</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>dwQ@g.com</t>
+          <t>prajwalsridhar1999@gmail.com</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>ds56</t>
+          <t>sgdf</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -478,22 +478,22 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>pramod</t>
+          <t>gt1</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>563456235263</t>
+          <t>hgsfz</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>prajwalsridhar1999@gmail.com</t>
+          <t>ghdsf@g.com</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>sgdf</t>
+          <t>dgsf</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -505,22 +505,22 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>gt</t>
+          <t>Prajwal S</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>hgsfz</t>
+          <t>07019660148</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>ghdsf@g.com</t>
+          <t>prajwalsridhar1999@gmail.com</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>dgsf</t>
+          <t>poiuy</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -532,22 +532,22 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>sudu</t>
+          <t>Prajwal S</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>26345342</t>
+          <t>07019660148</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>gd@gmail.com</t>
+          <t>prajwalsridhar1999@gmail.com</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>gdwfs</t>
+          <t>6557</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -559,12 +559,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Prajwal S</t>
+          <t>rak</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>07019660148</t>
+          <t>6345635</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -574,7 +574,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>hyt</t>
+          <t>ann</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -601,7 +601,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>poiuy</t>
+          <t>fd</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -613,7 +613,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Prajwal S</t>
+          <t>Prajwal S22</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -628,7 +628,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>poiuy</t>
+          <t>ds</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -640,12 +640,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Prajwal S</t>
+          <t>1</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>07019660148</t>
+          <t>1</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -655,93 +655,12 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>6557</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Shree photos sbm road maddur,mandya</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>rak</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>6345635</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>prajwalsridhar1999@gmail.com</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>ann</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>Shree photos sbm road maddur,mandya</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Prajwal S</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>07019660148</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>prajwalsridhar1999@gmail.com</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>fd</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>Shree photos sbm road maddur,mandya</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Prajwal S</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>07019660148</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>prajwalsridhar1999@gmail.com</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>pin</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>Shree photos sbm road maddur,mandya</t>
+          <t>1</t>
         </is>
       </c>
     </row>

</xml_diff>